<commit_message>
refactor the way messages are returned from the server. switch the rest of the app to use the oo rest call
</commit_message>
<xml_diff>
--- a/MMS200MI.xlsx
+++ b/MMS200MI.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="440">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="441">
   <si>
     <t>MMS200MI</t>
   </si>
@@ -24,6 +24,9 @@
     <t>CpyItmBasic</t>
   </si>
   <si>
+    <t>Result</t>
+  </si>
+  <si>
     <t>Company</t>
   </si>
   <si>
@@ -546,7 +549,7 @@
     <t>SPGV</t>
   </si>
   <si>
-    <t>CLAB1005GT</t>
+    <t>CLAB1TEST10</t>
   </si>
   <si>
     <t>Z95000</t>
@@ -567,13 +570,13 @@
     <t>Z95</t>
   </si>
   <si>
-    <t>CLAB1007GT</t>
+    <t>CLAB1TEST11</t>
   </si>
   <si>
     <t>50mL Mojonnier Flasks (each)</t>
   </si>
   <si>
-    <t>CLAB1008GT</t>
+    <t>CLAB1TEST12</t>
   </si>
   <si>
     <t>Stomacher Bags  (1000 pack)</t>
@@ -1467,24 +1470,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:CK65536"/>
+  <dimension ref="A1:CL7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5:C7"/>
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5:D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.2348178137652"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="10.6477732793522"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="12.2348178137652"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="10.6477732793522"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>1</v>
       </c>
@@ -1752,16 +1755,16 @@
         <v>88</v>
       </c>
       <c r="CJ3" s="0" t="s">
-        <v>4</v>
+        <v>89</v>
       </c>
       <c r="CK3" s="0" t="s">
-        <v>86</v>
+        <v>5</v>
+      </c>
+      <c r="CL3" s="0" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>89</v>
-      </c>
       <c r="B4" s="0" t="s">
         <v>90</v>
       </c>
@@ -2021,136 +2024,129 @@
         <v>175</v>
       </c>
       <c r="CJ4" s="0" t="s">
-        <v>91</v>
+        <v>176</v>
       </c>
       <c r="CK4" s="0" t="s">
-        <v>173</v>
+        <v>92</v>
+      </c>
+      <c r="CL4" s="0" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
+      <c r="B5" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="C5" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="2" t="s">
         <v>178</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="H5" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="G5" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="I5" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="J5" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="K5" s="4" t="n">
+      <c r="K5" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="L5" s="4" t="n">
         <v>9200</v>
       </c>
-      <c r="L5" s="4" t="n">
+      <c r="M5" s="4" t="n">
         <v>900</v>
       </c>
-      <c r="M5" s="2" t="s">
-        <v>182</v>
+      <c r="N5" s="2" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
+      <c r="B6" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="C6" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="L6" s="4" t="n">
+        <v>9200</v>
+      </c>
+      <c r="M6" s="4" t="n">
+        <v>900</v>
+      </c>
+      <c r="N6" s="2" t="s">
         <v>183</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="K6" s="4" t="n">
-        <v>9200</v>
-      </c>
-      <c r="L6" s="4" t="n">
-        <v>900</v>
-      </c>
-      <c r="M6" s="2" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
+      <c r="B7" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="C7" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="E7" s="3" t="s">
+      <c r="D7" s="1" t="s">
         <v>186</v>
       </c>
+      <c r="E7" s="2" t="s">
+        <v>178</v>
+      </c>
       <c r="F7" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="I7" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="I7" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="J7" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="K7" s="4" t="n">
+      <c r="K7" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="L7" s="4" t="n">
         <v>9200</v>
       </c>
-      <c r="L7" s="4" t="n">
+      <c r="M7" s="4" t="n">
         <v>900</v>
       </c>
-      <c r="M7" s="2" t="s">
-        <v>182</v>
+      <c r="N7" s="2" t="s">
+        <v>183</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
@@ -2167,10 +2163,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:ED7"/>
+  <dimension ref="A1:EE7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5:C7"/>
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -2185,7 +2181,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2193,13 +2189,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>188</v>
+        <v>3</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>4</v>
+        <v>189</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>189</v>
+        <v>5</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>190</v>
@@ -2271,10 +2267,10 @@
         <v>212</v>
       </c>
       <c r="AB3" s="0" t="s">
-        <v>9</v>
+        <v>213</v>
       </c>
       <c r="AC3" s="0" t="s">
-        <v>213</v>
+        <v>10</v>
       </c>
       <c r="AD3" s="0" t="s">
         <v>214</v>
@@ -2508,10 +2504,10 @@
         <v>290</v>
       </c>
       <c r="DC3" s="0" t="s">
-        <v>46</v>
+        <v>291</v>
       </c>
       <c r="DD3" s="0" t="s">
-        <v>291</v>
+        <v>47</v>
       </c>
       <c r="DE3" s="0" t="s">
         <v>292</v>
@@ -2529,22 +2525,22 @@
         <v>296</v>
       </c>
       <c r="DJ3" s="0" t="s">
-        <v>3</v>
+        <v>297</v>
       </c>
       <c r="DK3" s="0" t="s">
-        <v>69</v>
+        <v>4</v>
       </c>
       <c r="DL3" s="0" t="s">
         <v>70</v>
       </c>
       <c r="DM3" s="0" t="s">
-        <v>297</v>
+        <v>71</v>
       </c>
       <c r="DN3" s="0" t="s">
-        <v>72</v>
+        <v>298</v>
       </c>
       <c r="DO3" s="0" t="s">
-        <v>298</v>
+        <v>73</v>
       </c>
       <c r="DP3" s="0" t="s">
         <v>299</v>
@@ -2571,13 +2567,13 @@
         <v>306</v>
       </c>
       <c r="DX3" s="0" t="s">
-        <v>62</v>
+        <v>307</v>
       </c>
       <c r="DY3" s="0" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="DZ3" s="0" t="s">
-        <v>307</v>
+        <v>79</v>
       </c>
       <c r="EA3" s="0" t="s">
         <v>308</v>
@@ -2591,19 +2587,19 @@
       <c r="ED3" s="0" t="s">
         <v>311</v>
       </c>
+      <c r="EE3" s="0" t="s">
+        <v>312</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>89</v>
-      </c>
       <c r="B4" s="0" t="s">
-        <v>312</v>
+        <v>90</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>91</v>
+        <v>313</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>313</v>
+        <v>92</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>314</v>
@@ -2675,10 +2671,10 @@
         <v>336</v>
       </c>
       <c r="AB4" s="0" t="s">
-        <v>96</v>
+        <v>337</v>
       </c>
       <c r="AC4" s="0" t="s">
-        <v>337</v>
+        <v>97</v>
       </c>
       <c r="AD4" s="0" t="s">
         <v>338</v>
@@ -2912,10 +2908,10 @@
         <v>414</v>
       </c>
       <c r="DC4" s="0" t="s">
-        <v>133</v>
+        <v>415</v>
       </c>
       <c r="DD4" s="0" t="s">
-        <v>415</v>
+        <v>134</v>
       </c>
       <c r="DE4" s="0" t="s">
         <v>416</v>
@@ -2933,22 +2929,22 @@
         <v>420</v>
       </c>
       <c r="DJ4" s="0" t="s">
-        <v>90</v>
+        <v>421</v>
       </c>
       <c r="DK4" s="0" t="s">
-        <v>156</v>
+        <v>91</v>
       </c>
       <c r="DL4" s="0" t="s">
         <v>157</v>
       </c>
       <c r="DM4" s="0" t="s">
-        <v>421</v>
+        <v>158</v>
       </c>
       <c r="DN4" s="0" t="s">
-        <v>159</v>
+        <v>422</v>
       </c>
       <c r="DO4" s="0" t="s">
-        <v>422</v>
+        <v>160</v>
       </c>
       <c r="DP4" s="0" t="s">
         <v>423</v>
@@ -2978,10 +2974,10 @@
         <v>431</v>
       </c>
       <c r="DY4" s="0" t="s">
-        <v>165</v>
+        <v>432</v>
       </c>
       <c r="DZ4" s="0" t="s">
-        <v>432</v>
+        <v>166</v>
       </c>
       <c r="EA4" s="0" t="s">
         <v>433</v>
@@ -2995,71 +2991,74 @@
       <c r="ED4" s="0" t="s">
         <v>436</v>
       </c>
+      <c r="EE4" s="0" t="s">
+        <v>437</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
+      <c r="B5" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>437</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="AD5" s="1" t="n">
+      <c r="C5" s="2" t="s">
+        <v>438</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="AE5" s="1" t="n">
         <v>400658</v>
       </c>
-      <c r="AI5" s="1" t="s">
-        <v>438</v>
-      </c>
-      <c r="BA5" s="1" t="n">
+      <c r="AJ5" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="BB5" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="BX5" s="1" t="n">
+      <c r="BY5" s="1" t="n">
         <v>35</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
+      <c r="B6" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>437</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="AD6" s="1" t="n">
+      <c r="C6" s="2" t="s">
+        <v>438</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="AE6" s="1" t="n">
         <v>400658</v>
       </c>
-      <c r="AI6" s="1" t="s">
-        <v>439</v>
-      </c>
-      <c r="BA6" s="1"/>
-      <c r="BX6" s="1" t="n">
+      <c r="AJ6" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="BB6" s="1"/>
+      <c r="BY6" s="1" t="n">
         <v>42</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
+      <c r="B7" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>437</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="AD7" s="1" t="n">
+      <c r="C7" s="2" t="s">
+        <v>438</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="AE7" s="1" t="n">
         <v>400658</v>
       </c>
-      <c r="AI7" s="1" t="s">
-        <v>438</v>
-      </c>
-      <c r="BA7" s="1" t="n">
+      <c r="AJ7" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="BB7" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="BX7" s="1" t="n">
+      <c r="BY7" s="1" t="n">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
change the excel reading and processing to an object so i could better handle the error messaging
</commit_message>
<xml_diff>
--- a/MMS200MI.xlsx
+++ b/MMS200MI.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
-  <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
-  </bookViews>
-  <sheets>
-    <sheet name="MMS200MI_CpyItmBasic" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="MMS200MI_UpdItmWhs" sheetId="2" state="visible" r:id="rId3"/>
-  </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
-</workbook>
+<s:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <s:workbookPr codeName="ThisWorkbook"/>
+  <s:bookViews>
+    <s:workbookView activeTab="0"/>
+  </s:bookViews>
+  <s:sheets>
+    <s:sheet name="MMS200MI_CpyItmBasic" sheetId="1" r:id="rId1"/>
+    <s:sheet name="MMS200MI_CpyItmWhs" sheetId="2" r:id="rId2"/>
+    <s:sheet name="MMS200MI_UpdItmWhs" sheetId="3" r:id="rId3"/>
+  </s:sheets>
+  <s:definedNames/>
+  <s:calcPr calcId="124519" fullCalcOnLoad="1"/>
+</s:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="441">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="447">
   <si>
     <t>MMS200MI</t>
   </si>
@@ -549,7 +549,10 @@
     <t>SPGV</t>
   </si>
   <si>
-    <t>CLAB1TEST10</t>
+    <t xml:space="preserve">ServerReturnedNOK : A record has been entered by user JMIDDLETON XAD0001 </t>
+  </si>
+  <si>
+    <t>CLAB1TEST13</t>
   </si>
   <si>
     <t>Z95000</t>
@@ -570,18 +573,24 @@
     <t>Z95</t>
   </si>
   <si>
-    <t>CLAB1TEST11</t>
+    <t>CLAB1TEST14</t>
   </si>
   <si>
     <t>50mL Mojonnier Flasks (each)</t>
   </si>
   <si>
-    <t>CLAB1TEST12</t>
+    <t>CLAB1TEST15</t>
   </si>
   <si>
     <t>Stomacher Bags  (1000 pack)</t>
   </si>
   <si>
+    <t>CpyItmWhs</t>
+  </si>
+  <si>
+    <t>Transaction CpyItmWhs in program MMS200MI requires a value for field WHLO</t>
+  </si>
+  <si>
     <t>UpdItmWhs</t>
   </si>
   <si>
@@ -1332,13 +1341,22 @@
     <t>RMSG</t>
   </si>
   <si>
+    <t xml:space="preserve">ServerReturnedNOK : Item number CLAB1TEST13 does not exist WIT0103 </t>
+  </si>
+  <si>
     <t>1CO</t>
   </si>
   <si>
     <t>TEMPLATE</t>
   </si>
   <si>
+    <t xml:space="preserve">ServerReturnedNOK : Item number CLAB1TEST14 does not exist WIT0103 </t>
+  </si>
+  <si>
     <t>DISTRIBUTE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ServerReturnedNOK : Item number CLAB1TEST15 does not exist WIT0103 </t>
   </si>
 </sst>
 </file>
@@ -1346,55 +1364,52 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt formatCode="GENERAL" numFmtId="164"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
+      <name val="Calibri"/>
+      <charset val="1"/>
+      <family val="2"/>
+      <color rgb="FF000000"/>
       <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+      <color rgb="00000000"/>
+      <sz val="10"/>
     </font>
     <font>
-      <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+      <color rgb="00000000"/>
+      <sz val="10"/>
     </font>
     <font>
-      <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+      <color rgb="00000000"/>
+      <sz val="10"/>
     </font>
     <font>
+      <name val="Arial"/>
+      <charset val="1"/>
+      <family val="2"/>
+      <color rgb="FF000000"/>
       <sz val="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -1402,1673 +1417,3041 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+  <cellStyleXfs count="6">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="7">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="15">
+      <alignment horizontal="general" vertical="bottom"/>
     </xf>
-  </cellStyleXfs>
-  <cellXfs count="5">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="15">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="7">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
+  <cellStyles count="6">
+    <cellStyle builtinId="7" name="Currency [0]" xfId="0"/>
+    <cellStyle builtinId="3" name="Comma" xfId="1"/>
+    <cellStyle builtinId="5" name="Percent" xfId="2"/>
+    <cellStyle builtinId="6" name="Comma [0]" xfId="3"/>
+    <cellStyle builtinId="4" name="Currency" xfId="4"/>
+    <cellStyle builtinId="0" name="Normal" xfId="5"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr filterMode="0">
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:CL7"/>
+  <dimension ref="A1:GR13"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5:D7"/>
+    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A1" view="normal" windowProtection="0" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="D23" activeCellId="0" pane="topLeft" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="12.2348178137652"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="10.6477732793522"/>
+    <col customWidth="1" max="2" min="1" style="1" width="12.2348178137652"/>
+    <col customWidth="1" max="3" min="3" style="1" width="10.6477732793522"/>
+    <col customWidth="1" max="4" min="4" style="1" width="14.2186234817814"/>
+    <col customWidth="1" max="1025" min="5" style="1" width="10.6477732793522"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row customHeight="1" ht="13.8" r="1" s="6" spans="1:200">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="2" t="n"/>
+      <c r="C1" s="2" t="n"/>
+      <c r="D1" s="2" t="n"/>
+      <c r="E1" s="2" t="n"/>
+      <c r="F1" s="2" t="n"/>
+      <c r="G1" s="2" t="n"/>
+      <c r="H1" s="2" t="n"/>
+      <c r="I1" s="2" t="n"/>
+      <c r="J1" s="2" t="n"/>
+      <c r="K1" s="2" t="n"/>
+      <c r="L1" s="2" t="n"/>
+      <c r="M1" s="2" t="n"/>
+      <c r="N1" s="2" t="n"/>
+      <c r="O1" s="2" t="n"/>
+      <c r="P1" s="2" t="n"/>
+      <c r="Q1" s="2" t="n"/>
+      <c r="R1" s="2" t="n"/>
+      <c r="S1" s="2" t="n"/>
+      <c r="T1" s="2" t="n"/>
+      <c r="U1" s="2" t="n"/>
+      <c r="V1" s="2" t="n"/>
+      <c r="W1" s="2" t="n"/>
+      <c r="X1" s="2" t="n"/>
+      <c r="Y1" s="2" t="n"/>
+      <c r="Z1" s="2" t="n"/>
+      <c r="AA1" s="2" t="n"/>
+      <c r="AB1" s="2" t="n"/>
+      <c r="AC1" s="2" t="n"/>
+      <c r="AD1" s="2" t="n"/>
+      <c r="AE1" s="2" t="n"/>
+      <c r="AF1" s="2" t="n"/>
+      <c r="AG1" s="2" t="n"/>
+      <c r="AH1" s="2" t="n"/>
+      <c r="AI1" s="2" t="n"/>
+      <c r="AJ1" s="2" t="n"/>
+      <c r="AK1" s="2" t="n"/>
+      <c r="AL1" s="2" t="n"/>
+      <c r="AM1" s="2" t="n"/>
+      <c r="AN1" s="2" t="n"/>
+      <c r="AO1" s="2" t="n"/>
+      <c r="AP1" s="2" t="n"/>
+      <c r="AQ1" s="2" t="n"/>
+      <c r="AR1" s="2" t="n"/>
+      <c r="AS1" s="2" t="n"/>
+      <c r="AT1" s="2" t="n"/>
+      <c r="AU1" s="2" t="n"/>
+      <c r="AV1" s="2" t="n"/>
+      <c r="AW1" s="2" t="n"/>
+      <c r="AX1" s="2" t="n"/>
+      <c r="AY1" s="2" t="n"/>
+      <c r="AZ1" s="2" t="n"/>
+      <c r="BA1" s="2" t="n"/>
+      <c r="BB1" s="2" t="n"/>
+      <c r="BC1" s="2" t="n"/>
+      <c r="BD1" s="2" t="n"/>
+      <c r="BE1" s="2" t="n"/>
+      <c r="BF1" s="2" t="n"/>
+      <c r="BG1" s="2" t="n"/>
+      <c r="BH1" s="2" t="n"/>
+      <c r="BI1" s="2" t="n"/>
+      <c r="BJ1" s="2" t="n"/>
+      <c r="BK1" s="2" t="n"/>
+      <c r="BL1" s="2" t="n"/>
+      <c r="BM1" s="2" t="n"/>
+      <c r="BN1" s="2" t="n"/>
+      <c r="BO1" s="2" t="n"/>
+      <c r="BP1" s="2" t="n"/>
+      <c r="BQ1" s="2" t="n"/>
+      <c r="BR1" s="2" t="n"/>
+      <c r="BS1" s="2" t="n"/>
+      <c r="BT1" s="2" t="n"/>
+      <c r="BU1" s="2" t="n"/>
+      <c r="BV1" s="2" t="n"/>
+      <c r="BW1" s="2" t="n"/>
+      <c r="BX1" s="2" t="n"/>
+      <c r="BY1" s="2" t="n"/>
+      <c r="BZ1" s="2" t="n"/>
+      <c r="CA1" s="2" t="n"/>
+      <c r="CB1" s="2" t="n"/>
+      <c r="CC1" s="2" t="n"/>
+      <c r="CD1" s="2" t="n"/>
+      <c r="CE1" s="2" t="n"/>
+      <c r="CF1" s="2" t="n"/>
+      <c r="CG1" s="2" t="n"/>
+      <c r="CH1" s="2" t="n"/>
+      <c r="CI1" s="2" t="n"/>
+      <c r="CJ1" s="2" t="n"/>
+      <c r="CK1" s="2" t="n"/>
+      <c r="CL1" s="2" t="n"/>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+    <row customHeight="1" ht="13.8" r="2" s="6" spans="1:200">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="B2" s="2" t="n"/>
+      <c r="C2" s="2" t="n"/>
+      <c r="D2" s="2" t="n"/>
+      <c r="E2" s="2" t="n"/>
+      <c r="F2" s="2" t="n"/>
+      <c r="G2" s="2" t="n"/>
+      <c r="H2" s="2" t="n"/>
+      <c r="I2" s="2" t="n"/>
+      <c r="J2" s="2" t="n"/>
+      <c r="K2" s="2" t="n"/>
+      <c r="L2" s="2" t="n"/>
+      <c r="M2" s="2" t="n"/>
+      <c r="N2" s="2" t="n"/>
+      <c r="O2" s="2" t="n"/>
+      <c r="P2" s="2" t="n"/>
+      <c r="Q2" s="2" t="n"/>
+      <c r="R2" s="2" t="n"/>
+      <c r="S2" s="2" t="n"/>
+      <c r="T2" s="2" t="n"/>
+      <c r="U2" s="2" t="n"/>
+      <c r="V2" s="2" t="n"/>
+      <c r="W2" s="2" t="n"/>
+      <c r="X2" s="2" t="n"/>
+      <c r="Y2" s="2" t="n"/>
+      <c r="Z2" s="2" t="n"/>
+      <c r="AA2" s="2" t="n"/>
+      <c r="AB2" s="2" t="n"/>
+      <c r="AC2" s="2" t="n"/>
+      <c r="AD2" s="2" t="n"/>
+      <c r="AE2" s="2" t="n"/>
+      <c r="AF2" s="2" t="n"/>
+      <c r="AG2" s="2" t="n"/>
+      <c r="AH2" s="2" t="n"/>
+      <c r="AI2" s="2" t="n"/>
+      <c r="AJ2" s="2" t="n"/>
+      <c r="AK2" s="2" t="n"/>
+      <c r="AL2" s="2" t="n"/>
+      <c r="AM2" s="2" t="n"/>
+      <c r="AN2" s="2" t="n"/>
+      <c r="AO2" s="2" t="n"/>
+      <c r="AP2" s="2" t="n"/>
+      <c r="AQ2" s="2" t="n"/>
+      <c r="AR2" s="2" t="n"/>
+      <c r="AS2" s="2" t="n"/>
+      <c r="AT2" s="2" t="n"/>
+      <c r="AU2" s="2" t="n"/>
+      <c r="AV2" s="2" t="n"/>
+      <c r="AW2" s="2" t="n"/>
+      <c r="AX2" s="2" t="n"/>
+      <c r="AY2" s="2" t="n"/>
+      <c r="AZ2" s="2" t="n"/>
+      <c r="BA2" s="2" t="n"/>
+      <c r="BB2" s="2" t="n"/>
+      <c r="BC2" s="2" t="n"/>
+      <c r="BD2" s="2" t="n"/>
+      <c r="BE2" s="2" t="n"/>
+      <c r="BF2" s="2" t="n"/>
+      <c r="BG2" s="2" t="n"/>
+      <c r="BH2" s="2" t="n"/>
+      <c r="BI2" s="2" t="n"/>
+      <c r="BJ2" s="2" t="n"/>
+      <c r="BK2" s="2" t="n"/>
+      <c r="BL2" s="2" t="n"/>
+      <c r="BM2" s="2" t="n"/>
+      <c r="BN2" s="2" t="n"/>
+      <c r="BO2" s="2" t="n"/>
+      <c r="BP2" s="2" t="n"/>
+      <c r="BQ2" s="2" t="n"/>
+      <c r="BR2" s="2" t="n"/>
+      <c r="BS2" s="2" t="n"/>
+      <c r="BT2" s="2" t="n"/>
+      <c r="BU2" s="2" t="n"/>
+      <c r="BV2" s="2" t="n"/>
+      <c r="BW2" s="2" t="n"/>
+      <c r="BX2" s="2" t="n"/>
+      <c r="BY2" s="2" t="n"/>
+      <c r="BZ2" s="2" t="n"/>
+      <c r="CA2" s="2" t="n"/>
+      <c r="CB2" s="2" t="n"/>
+      <c r="CC2" s="2" t="n"/>
+      <c r="CD2" s="2" t="n"/>
+      <c r="CE2" s="2" t="n"/>
+      <c r="CF2" s="2" t="n"/>
+      <c r="CG2" s="2" t="n"/>
+      <c r="CH2" s="2" t="n"/>
+      <c r="CI2" s="2" t="n"/>
+      <c r="CJ2" s="2" t="n"/>
+      <c r="CK2" s="2" t="n"/>
+      <c r="CL2" s="2" t="n"/>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+    <row customHeight="1" ht="13.8" r="3" s="6" spans="1:200">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="F3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="0" t="s">
+      <c r="G3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="0" t="s">
+      <c r="H3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="0" t="s">
+      <c r="I3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="0" t="s">
+      <c r="J3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="K3" s="0" t="s">
+      <c r="K3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="L3" s="0" t="s">
+      <c r="L3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="M3" s="0" t="s">
+      <c r="M3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="N3" s="0" t="s">
+      <c r="N3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="O3" s="0" t="s">
+      <c r="O3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="P3" s="0" t="s">
+      <c r="P3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="Q3" s="0" t="s">
+      <c r="Q3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="R3" s="0" t="s">
+      <c r="R3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="S3" s="0" t="s">
+      <c r="S3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="T3" s="0" t="s">
+      <c r="T3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="U3" s="0" t="s">
+      <c r="U3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="V3" s="0" t="s">
+      <c r="V3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="W3" s="0" t="s">
+      <c r="W3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="X3" s="0" t="s">
+      <c r="X3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="Y3" s="0" t="s">
+      <c r="Y3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="Z3" s="0" t="s">
+      <c r="Z3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AA3" s="0" t="s">
+      <c r="AA3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AB3" s="0" t="s">
+      <c r="AB3" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AC3" s="0" t="s">
+      <c r="AC3" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AD3" s="0" t="s">
+      <c r="AD3" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="AE3" s="0" t="s">
+      <c r="AE3" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AF3" s="0" t="s">
+      <c r="AF3" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AG3" s="0" t="s">
+      <c r="AG3" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="AH3" s="0" t="s">
+      <c r="AH3" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AI3" s="0" t="s">
+      <c r="AI3" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="AJ3" s="0" t="s">
+      <c r="AJ3" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="AK3" s="0" t="s">
+      <c r="AK3" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="AL3" s="0" t="s">
+      <c r="AL3" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="AM3" s="0" t="s">
+      <c r="AM3" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AN3" s="0" t="s">
+      <c r="AN3" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="AO3" s="0" t="s">
+      <c r="AO3" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="AP3" s="0" t="s">
+      <c r="AP3" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="AQ3" s="0" t="s">
+      <c r="AQ3" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="AR3" s="0" t="s">
+      <c r="AR3" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="AS3" s="0" t="s">
+      <c r="AS3" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="AT3" s="0" t="s">
+      <c r="AT3" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="AU3" s="0" t="s">
+      <c r="AU3" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="AV3" s="0" t="s">
+      <c r="AV3" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="AW3" s="0" t="s">
+      <c r="AW3" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="AX3" s="0" t="s">
+      <c r="AX3" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="AY3" s="0" t="s">
+      <c r="AY3" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="AZ3" s="0" t="s">
+      <c r="AZ3" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="BA3" s="0" t="s">
+      <c r="BA3" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="BB3" s="0" t="s">
+      <c r="BB3" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="BC3" s="0" t="s">
+      <c r="BC3" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="BD3" s="0" t="s">
+      <c r="BD3" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="BE3" s="0" t="s">
+      <c r="BE3" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="BF3" s="0" t="s">
+      <c r="BF3" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="BG3" s="0" t="s">
+      <c r="BG3" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="BH3" s="0" t="s">
+      <c r="BH3" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="BI3" s="0" t="s">
+      <c r="BI3" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="BJ3" s="0" t="s">
+      <c r="BJ3" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="BK3" s="0" t="s">
+      <c r="BK3" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="BL3" s="0" t="s">
+      <c r="BL3" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="BM3" s="0" t="s">
+      <c r="BM3" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="BN3" s="0" t="s">
+      <c r="BN3" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="BO3" s="0" t="s">
+      <c r="BO3" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="BP3" s="0" t="s">
+      <c r="BP3" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="BQ3" s="0" t="s">
+      <c r="BQ3" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="BR3" s="0" t="s">
+      <c r="BR3" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="BS3" s="0" t="s">
+      <c r="BS3" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="BT3" s="0" t="s">
+      <c r="BT3" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="BU3" s="0" t="s">
+      <c r="BU3" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="BV3" s="0" t="s">
+      <c r="BV3" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="BW3" s="0" t="s">
+      <c r="BW3" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="BX3" s="0" t="s">
+      <c r="BX3" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="BY3" s="0" t="s">
+      <c r="BY3" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="BZ3" s="0" t="s">
+      <c r="BZ3" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="CA3" s="0" t="s">
+      <c r="CA3" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="CB3" s="0" t="s">
+      <c r="CB3" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="CC3" s="0" t="s">
+      <c r="CC3" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="CD3" s="0" t="s">
+      <c r="CD3" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="CE3" s="0" t="s">
+      <c r="CE3" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="CF3" s="0" t="s">
+      <c r="CF3" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="CG3" s="0" t="s">
+      <c r="CG3" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="CH3" s="0" t="s">
+      <c r="CH3" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="CI3" s="0" t="s">
+      <c r="CI3" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="CJ3" s="0" t="s">
+      <c r="CJ3" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="CK3" s="0" t="s">
+      <c r="CK3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="CL3" s="0" t="s">
+      <c r="CL3" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="0" t="s">
+    <row customHeight="1" ht="13.8" r="4" s="6" spans="1:200">
+      <c r="A4" s="2" t="n"/>
+      <c r="B4" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="E4" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="F4" s="0" t="s">
+      <c r="F4" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="G4" s="0" t="s">
+      <c r="G4" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="H4" s="0" t="s">
+      <c r="H4" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="I4" s="0" t="s">
+      <c r="I4" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="J4" s="0" t="s">
+      <c r="J4" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="K4" s="0" t="s">
+      <c r="K4" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="L4" s="0" t="s">
+      <c r="L4" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="M4" s="0" t="s">
+      <c r="M4" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="N4" s="0" t="s">
+      <c r="N4" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="O4" s="0" t="s">
+      <c r="O4" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="P4" s="0" t="s">
+      <c r="P4" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="Q4" s="0" t="s">
+      <c r="Q4" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="R4" s="0" t="s">
+      <c r="R4" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="S4" s="0" t="s">
+      <c r="S4" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="T4" s="0" t="s">
+      <c r="T4" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="U4" s="0" t="s">
+      <c r="U4" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="V4" s="0" t="s">
+      <c r="V4" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="W4" s="0" t="s">
+      <c r="W4" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="X4" s="0" t="s">
+      <c r="X4" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="Y4" s="0" t="s">
+      <c r="Y4" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="Z4" s="0" t="s">
+      <c r="Z4" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="AA4" s="0" t="s">
+      <c r="AA4" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="AB4" s="0" t="s">
+      <c r="AB4" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="AC4" s="0" t="s">
+      <c r="AC4" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="AD4" s="0" t="s">
+      <c r="AD4" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="AE4" s="0" t="s">
+      <c r="AE4" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="AF4" s="0" t="s">
+      <c r="AF4" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="AG4" s="0" t="s">
+      <c r="AG4" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="AH4" s="0" t="s">
+      <c r="AH4" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="AI4" s="0" t="s">
+      <c r="AI4" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="AJ4" s="0" t="s">
+      <c r="AJ4" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="AK4" s="0" t="s">
+      <c r="AK4" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="AL4" s="0" t="s">
+      <c r="AL4" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="AM4" s="0" t="s">
+      <c r="AM4" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="AN4" s="0" t="s">
+      <c r="AN4" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="AO4" s="0" t="s">
+      <c r="AO4" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="AP4" s="0" t="s">
+      <c r="AP4" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="AQ4" s="0" t="s">
+      <c r="AQ4" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="AR4" s="0" t="s">
+      <c r="AR4" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="AS4" s="0" t="s">
+      <c r="AS4" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="AT4" s="0" t="s">
+      <c r="AT4" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="AU4" s="0" t="s">
+      <c r="AU4" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="AV4" s="0" t="s">
+      <c r="AV4" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="AW4" s="0" t="s">
+      <c r="AW4" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="AX4" s="0" t="s">
+      <c r="AX4" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="AY4" s="0" t="s">
+      <c r="AY4" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="AZ4" s="0" t="s">
+      <c r="AZ4" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="BA4" s="0" t="s">
+      <c r="BA4" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="BB4" s="0" t="s">
+      <c r="BB4" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="BC4" s="0" t="s">
+      <c r="BC4" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="BD4" s="0" t="s">
+      <c r="BD4" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="BE4" s="0" t="s">
+      <c r="BE4" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="BF4" s="0" t="s">
+      <c r="BF4" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="BG4" s="0" t="s">
+      <c r="BG4" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="BH4" s="0" t="s">
+      <c r="BH4" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="BI4" s="0" t="s">
+      <c r="BI4" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="BJ4" s="0" t="s">
+      <c r="BJ4" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="BK4" s="0" t="s">
+      <c r="BK4" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="BL4" s="0" t="s">
+      <c r="BL4" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="BM4" s="0" t="s">
+      <c r="BM4" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="BN4" s="0" t="s">
+      <c r="BN4" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="BO4" s="0" t="s">
+      <c r="BO4" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="BP4" s="0" t="s">
+      <c r="BP4" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="BQ4" s="0" t="s">
+      <c r="BQ4" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="BR4" s="0" t="s">
+      <c r="BR4" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="BS4" s="0" t="s">
+      <c r="BS4" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="BT4" s="0" t="s">
+      <c r="BT4" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="BU4" s="0" t="s">
+      <c r="BU4" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="BV4" s="0" t="s">
+      <c r="BV4" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="BW4" s="0" t="s">
+      <c r="BW4" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="BX4" s="0" t="s">
+      <c r="BX4" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="BY4" s="0" t="s">
+      <c r="BY4" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="BZ4" s="0" t="s">
+      <c r="BZ4" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="CA4" s="0" t="s">
+      <c r="CA4" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="CB4" s="0" t="s">
+      <c r="CB4" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="CC4" s="0" t="s">
+      <c r="CC4" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="CD4" s="0" t="s">
+      <c r="CD4" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="CE4" s="0" t="s">
+      <c r="CE4" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="CF4" s="0" t="s">
+      <c r="CF4" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="CG4" s="0" t="s">
+      <c r="CG4" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="CH4" s="0" t="s">
+      <c r="CH4" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="CI4" s="0" t="s">
+      <c r="CI4" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="CJ4" s="0" t="s">
+      <c r="CJ4" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="CK4" s="0" t="s">
+      <c r="CK4" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="CL4" s="0" t="s">
+      <c r="CL4" s="2" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="0" t="n">
+    <row customHeight="1" ht="13.8" r="5" s="6" spans="1:200">
+      <c r="A5" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="B5" s="2" t="n">
         <v>100</v>
       </c>
-      <c r="C5" s="0" t="n">
+      <c r="C5" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="L5" s="5" t="n">
+        <v>9200</v>
+      </c>
+      <c r="M5" s="5" t="n">
+        <v>900</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="13.8" r="6" s="6" spans="1:200">
+      <c r="A6" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="B6" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="L6" s="5" t="n">
+        <v>9200</v>
+      </c>
+      <c r="M6" s="5" t="n">
+        <v>900</v>
+      </c>
+      <c r="N6" s="4" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="13.8" r="7" s="6" spans="1:200">
+      <c r="A7" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="B7" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="L7" s="5" t="n">
+        <v>9200</v>
+      </c>
+      <c r="M7" s="5" t="n">
+        <v>900</v>
+      </c>
+      <c r="N7" s="4" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="8" spans="1:200"/>
+    <row r="9" spans="1:200"/>
+    <row r="10" spans="1:200"/>
+    <row r="11" spans="1:200"/>
+    <row r="12" spans="1:200"/>
+    <row r="13" spans="1:200"/>
+  </sheetData>
+  <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageSetup blackAndWhite="0" copies="1" draft="0" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0" usePrinterDefaults="0" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr filterMode="0">
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr fitToPage="0"/>
+  </sheetPr>
+  <dimension ref="A1:GR13"/>
+  <sheetViews>
+    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="0" topLeftCell="A1" view="normal" windowProtection="0" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="D12" activeCellId="0" pane="topLeft" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col customWidth="1" max="3" min="1" style="2" width="9.1417004048583"/>
+    <col customWidth="1" max="4" min="4" style="2" width="16.2024291497976"/>
+    <col customWidth="1" max="1025" min="5" style="2" width="9.1417004048583"/>
+  </cols>
+  <sheetData>
+    <row customHeight="1" ht="13.8" r="1" s="6" spans="1:200">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="13.8" r="2" s="6" spans="1:200">
+      <c r="A2" s="2" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="13.8" r="3" s="6" spans="1:200">
+      <c r="B3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="U3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="V3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="W3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="X3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AD3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="AE3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AF3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AG3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="AH3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="AI3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AJ3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="AL3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="AM3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AN3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="AO3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AP3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AQ3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AR3" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="AS3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AT3" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="AU3" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="AV3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AW3" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AX3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AY3" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AZ3" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="BA3" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="BB3" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="BC3" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="BD3" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="BE3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BF3" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="BG3" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="BH3" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="BI3" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="BJ3" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="BK3" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="BL3" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="BM3" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="BN3" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="BO3" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="BP3" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="BQ3" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="BR3" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="BS3" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="BT3" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="BU3" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="BV3" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="BW3" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="BX3" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="BY3" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="BZ3" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="CA3" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="CB3" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="CC3" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="CD3" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="CE3" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="CF3" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="CG3" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="CH3" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="CI3" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="CJ3" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="CK3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="CL3" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="13.8" r="4" s="6" spans="1:200">
+      <c r="B4" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="T4" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="U4" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="V4" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="W4" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="X4" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="Y4" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="Z4" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AA4" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="AB4" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="AC4" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="AD4" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="AE4" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="AF4" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="AG4" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="AH4" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="AI4" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="AJ4" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="AK4" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="AL4" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="AM4" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="AN4" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="AO4" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="AP4" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="AQ4" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="AR4" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="AS4" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="AT4" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="AU4" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="AV4" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="AW4" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="AX4" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="AY4" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="AZ4" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="BA4" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="BB4" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="BC4" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="BD4" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="BE4" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="BF4" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="BG4" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="BH4" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="BI4" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="BJ4" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="BK4" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="BL4" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="BM4" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="BN4" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="BO4" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="BP4" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="BQ4" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="BR4" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="BS4" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="BT4" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="BU4" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="BV4" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="BW4" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="BX4" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="BY4" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="BZ4" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="CA4" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="CB4" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="CC4" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="CD4" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="CE4" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="CF4" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="CG4" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="CH4" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="CI4" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="CJ4" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="CK4" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="CL4" s="2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="13.8" r="5" s="6" spans="1:200">
+      <c r="A5" t="s">
+        <v>190</v>
+      </c>
+      <c r="B5" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="C5" s="4" t="n"/>
+      <c r="D5" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="E5" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="G5" s="3" t="s">
+    </row>
+    <row customHeight="1" ht="13.8" r="6" s="6" spans="1:200">
+      <c r="A6" t="s">
+        <v>190</v>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="C6" s="4" t="n"/>
+      <c r="D6" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="I5" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="L5" s="4" t="n">
-        <v>9200</v>
-      </c>
-      <c r="M5" s="4" t="n">
-        <v>900</v>
-      </c>
-      <c r="N5" s="2" t="s">
-        <v>183</v>
-      </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="0" t="n">
+    <row customHeight="1" ht="13.8" r="7" s="6" spans="1:200">
+      <c r="A7" t="s">
+        <v>190</v>
+      </c>
+      <c r="B7" s="2" t="n">
         <v>100</v>
       </c>
-      <c r="C6" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="L6" s="4" t="n">
-        <v>9200</v>
-      </c>
-      <c r="M6" s="4" t="n">
-        <v>900</v>
-      </c>
-      <c r="N6" s="2" t="s">
-        <v>183</v>
+      <c r="C7" s="4" t="n"/>
+      <c r="D7" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>179</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="C7" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="L7" s="4" t="n">
-        <v>9200</v>
-      </c>
-      <c r="M7" s="4" t="n">
-        <v>900</v>
-      </c>
-      <c r="N7" s="2" t="s">
-        <v>183</v>
-      </c>
-    </row>
+    <row r="8" spans="1:200"/>
+    <row r="9" spans="1:200"/>
+    <row r="10" spans="1:200"/>
+    <row r="11" spans="1:200"/>
+    <row r="12" spans="1:200"/>
+    <row r="13" spans="1:200"/>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
+  <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageSetup blackAndWhite="0" copies="1" draft="0" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0" usePrinterDefaults="0" verticalDpi="300"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;K000000&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;K000000Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr filterMode="0">
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:EE7"/>
+  <dimension ref="A1:GR13"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5:D7"/>
+    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="0" topLeftCell="A1" view="normal" windowProtection="0" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="E12" activeCellId="0" pane="topLeft" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.5910931174089"/>
+    <col customWidth="1" max="1025" min="1" style="1" width="10.5910931174089"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row customHeight="1" ht="13.8" r="1" s="6" spans="1:200">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="2" t="n"/>
+      <c r="C1" s="2" t="n"/>
+      <c r="D1" s="2" t="n"/>
+      <c r="E1" s="2" t="n"/>
+      <c r="F1" s="2" t="n"/>
+      <c r="G1" s="2" t="n"/>
+      <c r="H1" s="2" t="n"/>
+      <c r="I1" s="2" t="n"/>
+      <c r="J1" s="2" t="n"/>
+      <c r="K1" s="2" t="n"/>
+      <c r="L1" s="2" t="n"/>
+      <c r="M1" s="2" t="n"/>
+      <c r="N1" s="2" t="n"/>
+      <c r="O1" s="2" t="n"/>
+      <c r="P1" s="2" t="n"/>
+      <c r="Q1" s="2" t="n"/>
+      <c r="R1" s="2" t="n"/>
+      <c r="S1" s="2" t="n"/>
+      <c r="T1" s="2" t="n"/>
+      <c r="U1" s="2" t="n"/>
+      <c r="V1" s="2" t="n"/>
+      <c r="W1" s="2" t="n"/>
+      <c r="X1" s="2" t="n"/>
+      <c r="Y1" s="2" t="n"/>
+      <c r="Z1" s="2" t="n"/>
+      <c r="AA1" s="2" t="n"/>
+      <c r="AB1" s="2" t="n"/>
+      <c r="AC1" s="2" t="n"/>
+      <c r="AD1" s="2" t="n"/>
+      <c r="AE1" s="2" t="n"/>
+      <c r="AF1" s="2" t="n"/>
+      <c r="AG1" s="2" t="n"/>
+      <c r="AH1" s="2" t="n"/>
+      <c r="AI1" s="2" t="n"/>
+      <c r="AJ1" s="2" t="n"/>
+      <c r="AK1" s="2" t="n"/>
+      <c r="AL1" s="2" t="n"/>
+      <c r="AM1" s="2" t="n"/>
+      <c r="AN1" s="2" t="n"/>
+      <c r="AO1" s="2" t="n"/>
+      <c r="AP1" s="2" t="n"/>
+      <c r="AQ1" s="2" t="n"/>
+      <c r="AR1" s="2" t="n"/>
+      <c r="AS1" s="2" t="n"/>
+      <c r="AT1" s="2" t="n"/>
+      <c r="AU1" s="2" t="n"/>
+      <c r="AV1" s="2" t="n"/>
+      <c r="AW1" s="2" t="n"/>
+      <c r="AX1" s="2" t="n"/>
+      <c r="AY1" s="2" t="n"/>
+      <c r="AZ1" s="2" t="n"/>
+      <c r="BA1" s="2" t="n"/>
+      <c r="BB1" s="2" t="n"/>
+      <c r="BC1" s="2" t="n"/>
+      <c r="BD1" s="2" t="n"/>
+      <c r="BE1" s="2" t="n"/>
+      <c r="BF1" s="2" t="n"/>
+      <c r="BG1" s="2" t="n"/>
+      <c r="BH1" s="2" t="n"/>
+      <c r="BI1" s="2" t="n"/>
+      <c r="BJ1" s="2" t="n"/>
+      <c r="BK1" s="2" t="n"/>
+      <c r="BL1" s="2" t="n"/>
+      <c r="BM1" s="2" t="n"/>
+      <c r="BN1" s="2" t="n"/>
+      <c r="BO1" s="2" t="n"/>
+      <c r="BP1" s="2" t="n"/>
+      <c r="BQ1" s="2" t="n"/>
+      <c r="BR1" s="2" t="n"/>
+      <c r="BS1" s="2" t="n"/>
+      <c r="BT1" s="2" t="n"/>
+      <c r="BU1" s="2" t="n"/>
+      <c r="BV1" s="2" t="n"/>
+      <c r="BW1" s="2" t="n"/>
+      <c r="BX1" s="2" t="n"/>
+      <c r="BY1" s="2" t="n"/>
+      <c r="BZ1" s="2" t="n"/>
+      <c r="CA1" s="2" t="n"/>
+      <c r="CB1" s="2" t="n"/>
+      <c r="CC1" s="2" t="n"/>
+      <c r="CD1" s="2" t="n"/>
+      <c r="CE1" s="2" t="n"/>
+      <c r="CF1" s="2" t="n"/>
+      <c r="CG1" s="2" t="n"/>
+      <c r="CH1" s="2" t="n"/>
+      <c r="CI1" s="2" t="n"/>
+      <c r="CJ1" s="2" t="n"/>
+      <c r="CK1" s="2" t="n"/>
+      <c r="CL1" s="2" t="n"/>
+      <c r="CM1" s="2" t="n"/>
+      <c r="CN1" s="2" t="n"/>
+      <c r="CO1" s="2" t="n"/>
+      <c r="CP1" s="2" t="n"/>
+      <c r="CQ1" s="2" t="n"/>
+      <c r="CR1" s="2" t="n"/>
+      <c r="CS1" s="2" t="n"/>
+      <c r="CT1" s="2" t="n"/>
+      <c r="CU1" s="2" t="n"/>
+      <c r="CV1" s="2" t="n"/>
+      <c r="CW1" s="2" t="n"/>
+      <c r="CX1" s="2" t="n"/>
+      <c r="CY1" s="2" t="n"/>
+      <c r="CZ1" s="2" t="n"/>
+      <c r="DA1" s="2" t="n"/>
+      <c r="DB1" s="2" t="n"/>
+      <c r="DC1" s="2" t="n"/>
+      <c r="DD1" s="2" t="n"/>
+      <c r="DE1" s="2" t="n"/>
+      <c r="DF1" s="2" t="n"/>
+      <c r="DG1" s="2" t="n"/>
+      <c r="DH1" s="2" t="n"/>
+      <c r="DI1" s="2" t="n"/>
+      <c r="DJ1" s="2" t="n"/>
+      <c r="DK1" s="2" t="n"/>
+      <c r="DL1" s="2" t="n"/>
+      <c r="DM1" s="2" t="n"/>
+      <c r="DN1" s="2" t="n"/>
+      <c r="DO1" s="2" t="n"/>
+      <c r="DP1" s="2" t="n"/>
+      <c r="DQ1" s="2" t="n"/>
+      <c r="DR1" s="2" t="n"/>
+      <c r="DS1" s="2" t="n"/>
+      <c r="DT1" s="2" t="n"/>
+      <c r="DU1" s="2" t="n"/>
+      <c r="DV1" s="2" t="n"/>
+      <c r="DW1" s="2" t="n"/>
+      <c r="DX1" s="2" t="n"/>
+      <c r="DY1" s="2" t="n"/>
+      <c r="DZ1" s="2" t="n"/>
+      <c r="EA1" s="2" t="n"/>
+      <c r="EB1" s="2" t="n"/>
+      <c r="EC1" s="2" t="n"/>
+      <c r="ED1" s="2" t="n"/>
+      <c r="EE1" s="2" t="n"/>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>188</v>
-      </c>
+    <row customHeight="1" ht="13.8" r="2" s="6" spans="1:200">
+      <c r="A2" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B2" s="2" t="n"/>
+      <c r="C2" s="2" t="n"/>
+      <c r="D2" s="2" t="n"/>
+      <c r="E2" s="2" t="n"/>
+      <c r="F2" s="2" t="n"/>
+      <c r="G2" s="2" t="n"/>
+      <c r="H2" s="2" t="n"/>
+      <c r="I2" s="2" t="n"/>
+      <c r="J2" s="2" t="n"/>
+      <c r="K2" s="2" t="n"/>
+      <c r="L2" s="2" t="n"/>
+      <c r="M2" s="2" t="n"/>
+      <c r="N2" s="2" t="n"/>
+      <c r="O2" s="2" t="n"/>
+      <c r="P2" s="2" t="n"/>
+      <c r="Q2" s="2" t="n"/>
+      <c r="R2" s="2" t="n"/>
+      <c r="S2" s="2" t="n"/>
+      <c r="T2" s="2" t="n"/>
+      <c r="U2" s="2" t="n"/>
+      <c r="V2" s="2" t="n"/>
+      <c r="W2" s="2" t="n"/>
+      <c r="X2" s="2" t="n"/>
+      <c r="Y2" s="2" t="n"/>
+      <c r="Z2" s="2" t="n"/>
+      <c r="AA2" s="2" t="n"/>
+      <c r="AB2" s="2" t="n"/>
+      <c r="AC2" s="2" t="n"/>
+      <c r="AD2" s="2" t="n"/>
+      <c r="AE2" s="2" t="n"/>
+      <c r="AF2" s="2" t="n"/>
+      <c r="AG2" s="2" t="n"/>
+      <c r="AH2" s="2" t="n"/>
+      <c r="AI2" s="2" t="n"/>
+      <c r="AJ2" s="2" t="n"/>
+      <c r="AK2" s="2" t="n"/>
+      <c r="AL2" s="2" t="n"/>
+      <c r="AM2" s="2" t="n"/>
+      <c r="AN2" s="2" t="n"/>
+      <c r="AO2" s="2" t="n"/>
+      <c r="AP2" s="2" t="n"/>
+      <c r="AQ2" s="2" t="n"/>
+      <c r="AR2" s="2" t="n"/>
+      <c r="AS2" s="2" t="n"/>
+      <c r="AT2" s="2" t="n"/>
+      <c r="AU2" s="2" t="n"/>
+      <c r="AV2" s="2" t="n"/>
+      <c r="AW2" s="2" t="n"/>
+      <c r="AX2" s="2" t="n"/>
+      <c r="AY2" s="2" t="n"/>
+      <c r="AZ2" s="2" t="n"/>
+      <c r="BA2" s="2" t="n"/>
+      <c r="BB2" s="2" t="n"/>
+      <c r="BC2" s="2" t="n"/>
+      <c r="BD2" s="2" t="n"/>
+      <c r="BE2" s="2" t="n"/>
+      <c r="BF2" s="2" t="n"/>
+      <c r="BG2" s="2" t="n"/>
+      <c r="BH2" s="2" t="n"/>
+      <c r="BI2" s="2" t="n"/>
+      <c r="BJ2" s="2" t="n"/>
+      <c r="BK2" s="2" t="n"/>
+      <c r="BL2" s="2" t="n"/>
+      <c r="BM2" s="2" t="n"/>
+      <c r="BN2" s="2" t="n"/>
+      <c r="BO2" s="2" t="n"/>
+      <c r="BP2" s="2" t="n"/>
+      <c r="BQ2" s="2" t="n"/>
+      <c r="BR2" s="2" t="n"/>
+      <c r="BS2" s="2" t="n"/>
+      <c r="BT2" s="2" t="n"/>
+      <c r="BU2" s="2" t="n"/>
+      <c r="BV2" s="2" t="n"/>
+      <c r="BW2" s="2" t="n"/>
+      <c r="BX2" s="2" t="n"/>
+      <c r="BY2" s="2" t="n"/>
+      <c r="BZ2" s="2" t="n"/>
+      <c r="CA2" s="2" t="n"/>
+      <c r="CB2" s="2" t="n"/>
+      <c r="CC2" s="2" t="n"/>
+      <c r="CD2" s="2" t="n"/>
+      <c r="CE2" s="2" t="n"/>
+      <c r="CF2" s="2" t="n"/>
+      <c r="CG2" s="2" t="n"/>
+      <c r="CH2" s="2" t="n"/>
+      <c r="CI2" s="2" t="n"/>
+      <c r="CJ2" s="2" t="n"/>
+      <c r="CK2" s="2" t="n"/>
+      <c r="CL2" s="2" t="n"/>
+      <c r="CM2" s="2" t="n"/>
+      <c r="CN2" s="2" t="n"/>
+      <c r="CO2" s="2" t="n"/>
+      <c r="CP2" s="2" t="n"/>
+      <c r="CQ2" s="2" t="n"/>
+      <c r="CR2" s="2" t="n"/>
+      <c r="CS2" s="2" t="n"/>
+      <c r="CT2" s="2" t="n"/>
+      <c r="CU2" s="2" t="n"/>
+      <c r="CV2" s="2" t="n"/>
+      <c r="CW2" s="2" t="n"/>
+      <c r="CX2" s="2" t="n"/>
+      <c r="CY2" s="2" t="n"/>
+      <c r="CZ2" s="2" t="n"/>
+      <c r="DA2" s="2" t="n"/>
+      <c r="DB2" s="2" t="n"/>
+      <c r="DC2" s="2" t="n"/>
+      <c r="DD2" s="2" t="n"/>
+      <c r="DE2" s="2" t="n"/>
+      <c r="DF2" s="2" t="n"/>
+      <c r="DG2" s="2" t="n"/>
+      <c r="DH2" s="2" t="n"/>
+      <c r="DI2" s="2" t="n"/>
+      <c r="DJ2" s="2" t="n"/>
+      <c r="DK2" s="2" t="n"/>
+      <c r="DL2" s="2" t="n"/>
+      <c r="DM2" s="2" t="n"/>
+      <c r="DN2" s="2" t="n"/>
+      <c r="DO2" s="2" t="n"/>
+      <c r="DP2" s="2" t="n"/>
+      <c r="DQ2" s="2" t="n"/>
+      <c r="DR2" s="2" t="n"/>
+      <c r="DS2" s="2" t="n"/>
+      <c r="DT2" s="2" t="n"/>
+      <c r="DU2" s="2" t="n"/>
+      <c r="DV2" s="2" t="n"/>
+      <c r="DW2" s="2" t="n"/>
+      <c r="DX2" s="2" t="n"/>
+      <c r="DY2" s="2" t="n"/>
+      <c r="DZ2" s="2" t="n"/>
+      <c r="EA2" s="2" t="n"/>
+      <c r="EB2" s="2" t="n"/>
+      <c r="EC2" s="2" t="n"/>
+      <c r="ED2" s="2" t="n"/>
+      <c r="EE2" s="2" t="n"/>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+    <row customHeight="1" ht="13.8" r="3" s="6" spans="1:200">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="0" t="s">
-        <v>189</v>
-      </c>
-      <c r="D3" s="0" t="s">
+      <c r="C3" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="0" t="s">
-        <v>190</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>191</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>192</v>
-      </c>
-      <c r="H3" s="0" t="s">
+      <c r="E3" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="I3" s="0" t="s">
+      <c r="F3" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="J3" s="0" t="s">
+      <c r="G3" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="K3" s="0" t="s">
+      <c r="H3" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="L3" s="0" t="s">
+      <c r="I3" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="M3" s="0" t="s">
+      <c r="J3" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="N3" s="0" t="s">
+      <c r="K3" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="O3" s="0" t="s">
+      <c r="L3" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="P3" s="0" t="s">
+      <c r="M3" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="Q3" s="0" t="s">
+      <c r="N3" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="R3" s="0" t="s">
+      <c r="O3" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="S3" s="0" t="s">
+      <c r="P3" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="T3" s="0" t="s">
+      <c r="Q3" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="U3" s="0" t="s">
+      <c r="R3" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="V3" s="0" t="s">
+      <c r="S3" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="W3" s="0" t="s">
+      <c r="T3" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="X3" s="0" t="s">
+      <c r="U3" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="Y3" s="0" t="s">
+      <c r="V3" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="Z3" s="0" t="s">
+      <c r="W3" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="AA3" s="0" t="s">
+      <c r="X3" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="AB3" s="0" t="s">
+      <c r="Y3" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="AC3" s="0" t="s">
+      <c r="Z3" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="AA3" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="AB3" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="AC3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="AD3" s="0" t="s">
-        <v>214</v>
-      </c>
-      <c r="AE3" s="0" t="s">
-        <v>215</v>
-      </c>
-      <c r="AF3" s="0" t="s">
-        <v>216</v>
-      </c>
-      <c r="AG3" s="0" t="s">
+      <c r="AD3" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="AH3" s="0" t="s">
+      <c r="AE3" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="AI3" s="0" t="s">
+      <c r="AF3" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="AJ3" s="0" t="s">
+      <c r="AG3" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="AK3" s="0" t="s">
+      <c r="AH3" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="AL3" s="0" t="s">
+      <c r="AI3" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="AM3" s="0" t="s">
+      <c r="AJ3" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="AN3" s="0" t="s">
+      <c r="AK3" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="AO3" s="0" t="s">
+      <c r="AL3" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="AP3" s="0" t="s">
+      <c r="AM3" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="AQ3" s="0" t="s">
+      <c r="AN3" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="AR3" s="0" t="s">
+      <c r="AO3" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="AS3" s="0" t="s">
+      <c r="AP3" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="AT3" s="0" t="s">
+      <c r="AQ3" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="AU3" s="0" t="s">
+      <c r="AR3" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="AV3" s="0" t="s">
+      <c r="AS3" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="AW3" s="0" t="s">
+      <c r="AT3" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="AX3" s="0" t="s">
+      <c r="AU3" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="AY3" s="0" t="s">
+      <c r="AV3" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="AZ3" s="0" t="s">
+      <c r="AW3" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="BA3" s="0" t="s">
+      <c r="AX3" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="BB3" s="0" t="s">
+      <c r="AY3" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="BC3" s="0" t="s">
+      <c r="AZ3" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="BD3" s="0" t="s">
+      <c r="BA3" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="BE3" s="0" t="s">
+      <c r="BB3" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="BF3" s="0" t="s">
+      <c r="BC3" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="BG3" s="0" t="s">
+      <c r="BD3" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="BH3" s="0" t="s">
+      <c r="BE3" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="BI3" s="0" t="s">
+      <c r="BF3" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="BJ3" s="0" t="s">
+      <c r="BG3" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="BK3" s="0" t="s">
+      <c r="BH3" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="BL3" s="0" t="s">
+      <c r="BI3" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="BM3" s="0" t="s">
+      <c r="BJ3" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="BN3" s="0" t="s">
+      <c r="BK3" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="BO3" s="0" t="s">
+      <c r="BL3" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="BP3" s="0" t="s">
+      <c r="BM3" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="BQ3" s="0" t="s">
+      <c r="BN3" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="BR3" s="0" t="s">
+      <c r="BO3" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="BS3" s="0" t="s">
+      <c r="BP3" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="BT3" s="0" t="s">
+      <c r="BQ3" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="BU3" s="0" t="s">
+      <c r="BR3" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="BV3" s="0" t="s">
+      <c r="BS3" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="BW3" s="0" t="s">
+      <c r="BT3" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="BX3" s="0" t="s">
+      <c r="BU3" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="BY3" s="0" t="s">
+      <c r="BV3" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="BZ3" s="0" t="s">
+      <c r="BW3" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="CA3" s="0" t="s">
+      <c r="BX3" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="CB3" s="0" t="s">
+      <c r="BY3" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="CC3" s="0" t="s">
+      <c r="BZ3" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="CD3" s="0" t="s">
+      <c r="CA3" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="CE3" s="0" t="s">
+      <c r="CB3" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="CF3" s="0" t="s">
+      <c r="CC3" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="CG3" s="0" t="s">
+      <c r="CD3" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="CH3" s="0" t="s">
+      <c r="CE3" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="CI3" s="0" t="s">
+      <c r="CF3" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="CJ3" s="0" t="s">
+      <c r="CG3" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="CK3" s="0" t="s">
+      <c r="CH3" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="CL3" s="0" t="s">
+      <c r="CI3" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="CM3" s="0" t="s">
+      <c r="CJ3" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="CN3" s="0" t="s">
+      <c r="CK3" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="CO3" s="0" t="s">
+      <c r="CL3" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="CP3" s="0" t="s">
+      <c r="CM3" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="CQ3" s="0" t="s">
+      <c r="CN3" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="CR3" s="0" t="s">
+      <c r="CO3" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="CS3" s="0" t="s">
+      <c r="CP3" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="CT3" s="0" t="s">
+      <c r="CQ3" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="CU3" s="0" t="s">
+      <c r="CR3" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="CV3" s="0" t="s">
+      <c r="CS3" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="CW3" s="0" t="s">
+      <c r="CT3" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="CX3" s="0" t="s">
+      <c r="CU3" s="2" t="s">
         <v>286</v>
       </c>
-      <c r="CY3" s="0" t="s">
+      <c r="CV3" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="CZ3" s="0" t="s">
+      <c r="CW3" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="DA3" s="0" t="s">
+      <c r="CX3" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="DB3" s="0" t="s">
+      <c r="CY3" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="DC3" s="0" t="s">
+      <c r="CZ3" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="DD3" s="0" t="s">
+      <c r="DA3" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="DB3" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="DC3" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="DD3" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="DE3" s="0" t="s">
-        <v>292</v>
-      </c>
-      <c r="DF3" s="0" t="s">
-        <v>293</v>
-      </c>
-      <c r="DG3" s="0" t="s">
-        <v>294</v>
-      </c>
-      <c r="DH3" s="0" t="s">
+      <c r="DE3" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="DI3" s="0" t="s">
+      <c r="DF3" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="DJ3" s="0" t="s">
+      <c r="DG3" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="DK3" s="0" t="s">
+      <c r="DH3" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="DI3" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="DJ3" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="DK3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="DL3" s="0" t="s">
+      <c r="DL3" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="DM3" s="0" t="s">
+      <c r="DM3" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="DN3" s="0" t="s">
-        <v>298</v>
-      </c>
-      <c r="DO3" s="0" t="s">
+      <c r="DN3" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="DO3" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="DP3" s="0" t="s">
-        <v>299</v>
-      </c>
-      <c r="DQ3" s="0" t="s">
-        <v>300</v>
-      </c>
-      <c r="DR3" s="0" t="s">
-        <v>301</v>
-      </c>
-      <c r="DS3" s="0" t="s">
+      <c r="DP3" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="DT3" s="0" t="s">
+      <c r="DQ3" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="DU3" s="0" t="s">
+      <c r="DR3" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="DV3" s="0" t="s">
+      <c r="DS3" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="DW3" s="0" t="s">
+      <c r="DT3" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="DX3" s="0" t="s">
+      <c r="DU3" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="DY3" s="0" t="s">
+      <c r="DV3" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="DW3" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="DX3" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="DY3" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="DZ3" s="0" t="s">
+      <c r="DZ3" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="EA3" s="0" t="s">
-        <v>308</v>
-      </c>
-      <c r="EB3" s="0" t="s">
-        <v>309</v>
-      </c>
-      <c r="EC3" s="0" t="s">
-        <v>310</v>
-      </c>
-      <c r="ED3" s="0" t="s">
+      <c r="EA3" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="EE3" s="0" t="s">
+      <c r="EB3" s="2" t="s">
         <v>312</v>
       </c>
+      <c r="EC3" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="ED3" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="EE3" s="2" t="s">
+        <v>315</v>
+      </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="0" t="s">
+    <row customHeight="1" ht="13.8" r="4" s="6" spans="1:200">
+      <c r="B4" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="C4" s="0" t="s">
-        <v>313</v>
-      </c>
-      <c r="D4" s="0" t="s">
+      <c r="C4" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="E4" s="0" t="s">
-        <v>314</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>315</v>
-      </c>
-      <c r="G4" s="0" t="s">
-        <v>316</v>
-      </c>
-      <c r="H4" s="0" t="s">
+      <c r="E4" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="I4" s="0" t="s">
+      <c r="F4" s="2" t="s">
         <v>318</v>
       </c>
-      <c r="J4" s="0" t="s">
+      <c r="G4" s="2" t="s">
         <v>319</v>
       </c>
-      <c r="K4" s="0" t="s">
+      <c r="H4" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="L4" s="0" t="s">
+      <c r="I4" s="2" t="s">
         <v>321</v>
       </c>
-      <c r="M4" s="0" t="s">
+      <c r="J4" s="2" t="s">
         <v>322</v>
       </c>
-      <c r="N4" s="0" t="s">
+      <c r="K4" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="O4" s="0" t="s">
+      <c r="L4" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="P4" s="0" t="s">
+      <c r="M4" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="Q4" s="0" t="s">
+      <c r="N4" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="R4" s="0" t="s">
+      <c r="O4" s="2" t="s">
         <v>327</v>
       </c>
-      <c r="S4" s="0" t="s">
+      <c r="P4" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="T4" s="0" t="s">
+      <c r="Q4" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="U4" s="0" t="s">
+      <c r="R4" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="V4" s="0" t="s">
+      <c r="S4" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="W4" s="0" t="s">
+      <c r="T4" s="2" t="s">
         <v>332</v>
       </c>
-      <c r="X4" s="0" t="s">
+      <c r="U4" s="2" t="s">
         <v>333</v>
       </c>
-      <c r="Y4" s="0" t="s">
+      <c r="V4" s="2" t="s">
         <v>334</v>
       </c>
-      <c r="Z4" s="0" t="s">
+      <c r="W4" s="2" t="s">
         <v>335</v>
       </c>
-      <c r="AA4" s="0" t="s">
+      <c r="X4" s="2" t="s">
         <v>336</v>
       </c>
-      <c r="AB4" s="0" t="s">
+      <c r="Y4" s="2" t="s">
         <v>337</v>
       </c>
-      <c r="AC4" s="0" t="s">
+      <c r="Z4" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="AA4" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="AB4" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="AC4" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="AD4" s="0" t="s">
-        <v>338</v>
-      </c>
-      <c r="AE4" s="0" t="s">
-        <v>339</v>
-      </c>
-      <c r="AF4" s="0" t="s">
-        <v>340</v>
-      </c>
-      <c r="AG4" s="0" t="s">
+      <c r="AD4" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="AH4" s="0" t="s">
+      <c r="AE4" s="2" t="s">
         <v>342</v>
       </c>
-      <c r="AI4" s="0" t="s">
+      <c r="AF4" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="AJ4" s="0" t="s">
+      <c r="AG4" s="2" t="s">
         <v>344</v>
       </c>
-      <c r="AK4" s="0" t="s">
+      <c r="AH4" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="AL4" s="0" t="s">
+      <c r="AI4" s="2" t="s">
         <v>346</v>
       </c>
-      <c r="AM4" s="0" t="s">
+      <c r="AJ4" s="2" t="s">
         <v>347</v>
       </c>
-      <c r="AN4" s="0" t="s">
+      <c r="AK4" s="2" t="s">
         <v>348</v>
       </c>
-      <c r="AO4" s="0" t="s">
+      <c r="AL4" s="2" t="s">
         <v>349</v>
       </c>
-      <c r="AP4" s="0" t="s">
+      <c r="AM4" s="2" t="s">
         <v>350</v>
       </c>
-      <c r="AQ4" s="0" t="s">
+      <c r="AN4" s="2" t="s">
         <v>351</v>
       </c>
-      <c r="AR4" s="0" t="s">
+      <c r="AO4" s="2" t="s">
         <v>352</v>
       </c>
-      <c r="AS4" s="0" t="s">
+      <c r="AP4" s="2" t="s">
         <v>353</v>
       </c>
-      <c r="AT4" s="0" t="s">
+      <c r="AQ4" s="2" t="s">
         <v>354</v>
       </c>
-      <c r="AU4" s="0" t="s">
+      <c r="AR4" s="2" t="s">
         <v>355</v>
       </c>
-      <c r="AV4" s="0" t="s">
+      <c r="AS4" s="2" t="s">
         <v>356</v>
       </c>
-      <c r="AW4" s="0" t="s">
+      <c r="AT4" s="2" t="s">
         <v>357</v>
       </c>
-      <c r="AX4" s="0" t="s">
+      <c r="AU4" s="2" t="s">
         <v>358</v>
       </c>
-      <c r="AY4" s="0" t="s">
+      <c r="AV4" s="2" t="s">
         <v>359</v>
       </c>
-      <c r="AZ4" s="0" t="s">
+      <c r="AW4" s="2" t="s">
         <v>360</v>
       </c>
-      <c r="BA4" s="0" t="s">
+      <c r="AX4" s="2" t="s">
         <v>361</v>
       </c>
-      <c r="BB4" s="0" t="s">
+      <c r="AY4" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="BC4" s="0" t="s">
+      <c r="AZ4" s="2" t="s">
         <v>363</v>
       </c>
-      <c r="BD4" s="0" t="s">
+      <c r="BA4" s="2" t="s">
         <v>364</v>
       </c>
-      <c r="BE4" s="0" t="s">
+      <c r="BB4" s="2" t="s">
         <v>365</v>
       </c>
-      <c r="BF4" s="0" t="s">
+      <c r="BC4" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="BG4" s="0" t="s">
+      <c r="BD4" s="2" t="s">
         <v>367</v>
       </c>
-      <c r="BH4" s="0" t="s">
+      <c r="BE4" s="2" t="s">
         <v>368</v>
       </c>
-      <c r="BI4" s="0" t="s">
+      <c r="BF4" s="2" t="s">
         <v>369</v>
       </c>
-      <c r="BJ4" s="0" t="s">
+      <c r="BG4" s="2" t="s">
         <v>370</v>
       </c>
-      <c r="BK4" s="0" t="s">
+      <c r="BH4" s="2" t="s">
         <v>371</v>
       </c>
-      <c r="BL4" s="0" t="s">
+      <c r="BI4" s="2" t="s">
         <v>372</v>
       </c>
-      <c r="BM4" s="0" t="s">
+      <c r="BJ4" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="BN4" s="0" t="s">
+      <c r="BK4" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="BO4" s="0" t="s">
+      <c r="BL4" s="2" t="s">
         <v>375</v>
       </c>
-      <c r="BP4" s="0" t="s">
+      <c r="BM4" s="2" t="s">
         <v>376</v>
       </c>
-      <c r="BQ4" s="0" t="s">
+      <c r="BN4" s="2" t="s">
         <v>377</v>
       </c>
-      <c r="BR4" s="0" t="s">
+      <c r="BO4" s="2" t="s">
         <v>378</v>
       </c>
-      <c r="BS4" s="0" t="s">
+      <c r="BP4" s="2" t="s">
         <v>379</v>
       </c>
-      <c r="BT4" s="0" t="s">
+      <c r="BQ4" s="2" t="s">
         <v>380</v>
       </c>
-      <c r="BU4" s="0" t="s">
+      <c r="BR4" s="2" t="s">
         <v>381</v>
       </c>
-      <c r="BV4" s="0" t="s">
+      <c r="BS4" s="2" t="s">
         <v>382</v>
       </c>
-      <c r="BW4" s="0" t="s">
+      <c r="BT4" s="2" t="s">
         <v>383</v>
       </c>
-      <c r="BX4" s="0" t="s">
+      <c r="BU4" s="2" t="s">
         <v>384</v>
       </c>
-      <c r="BY4" s="0" t="s">
+      <c r="BV4" s="2" t="s">
         <v>385</v>
       </c>
-      <c r="BZ4" s="0" t="s">
+      <c r="BW4" s="2" t="s">
         <v>386</v>
       </c>
-      <c r="CA4" s="0" t="s">
+      <c r="BX4" s="2" t="s">
         <v>387</v>
       </c>
-      <c r="CB4" s="0" t="s">
+      <c r="BY4" s="2" t="s">
         <v>388</v>
       </c>
-      <c r="CC4" s="0" t="s">
+      <c r="BZ4" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="CD4" s="0" t="s">
+      <c r="CA4" s="2" t="s">
         <v>390</v>
       </c>
-      <c r="CE4" s="0" t="s">
+      <c r="CB4" s="2" t="s">
         <v>391</v>
       </c>
-      <c r="CF4" s="0" t="s">
+      <c r="CC4" s="2" t="s">
         <v>392</v>
       </c>
-      <c r="CG4" s="0" t="s">
+      <c r="CD4" s="2" t="s">
         <v>393</v>
       </c>
-      <c r="CH4" s="0" t="s">
+      <c r="CE4" s="2" t="s">
         <v>394</v>
       </c>
-      <c r="CI4" s="0" t="s">
+      <c r="CF4" s="2" t="s">
         <v>395</v>
       </c>
-      <c r="CJ4" s="0" t="s">
+      <c r="CG4" s="2" t="s">
         <v>396</v>
       </c>
-      <c r="CK4" s="0" t="s">
+      <c r="CH4" s="2" t="s">
         <v>397</v>
       </c>
-      <c r="CL4" s="0" t="s">
+      <c r="CI4" s="2" t="s">
         <v>398</v>
       </c>
-      <c r="CM4" s="0" t="s">
+      <c r="CJ4" s="2" t="s">
         <v>399</v>
       </c>
-      <c r="CN4" s="0" t="s">
+      <c r="CK4" s="2" t="s">
         <v>400</v>
       </c>
-      <c r="CO4" s="0" t="s">
+      <c r="CL4" s="2" t="s">
         <v>401</v>
       </c>
-      <c r="CP4" s="0" t="s">
+      <c r="CM4" s="2" t="s">
         <v>402</v>
       </c>
-      <c r="CQ4" s="0" t="s">
+      <c r="CN4" s="2" t="s">
         <v>403</v>
       </c>
-      <c r="CR4" s="0" t="s">
+      <c r="CO4" s="2" t="s">
         <v>404</v>
       </c>
-      <c r="CS4" s="0" t="s">
+      <c r="CP4" s="2" t="s">
         <v>405</v>
       </c>
-      <c r="CT4" s="0" t="s">
+      <c r="CQ4" s="2" t="s">
         <v>406</v>
       </c>
-      <c r="CU4" s="0" t="s">
+      <c r="CR4" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="CV4" s="0" t="s">
+      <c r="CS4" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="CW4" s="0" t="s">
+      <c r="CT4" s="2" t="s">
         <v>409</v>
       </c>
-      <c r="CX4" s="0" t="s">
+      <c r="CU4" s="2" t="s">
         <v>410</v>
       </c>
-      <c r="CY4" s="0" t="s">
+      <c r="CV4" s="2" t="s">
         <v>411</v>
       </c>
-      <c r="CZ4" s="0" t="s">
+      <c r="CW4" s="2" t="s">
         <v>412</v>
       </c>
-      <c r="DA4" s="0" t="s">
+      <c r="CX4" s="2" t="s">
         <v>413</v>
       </c>
-      <c r="DB4" s="0" t="s">
+      <c r="CY4" s="2" t="s">
         <v>414</v>
       </c>
-      <c r="DC4" s="0" t="s">
+      <c r="CZ4" s="2" t="s">
         <v>415</v>
       </c>
-      <c r="DD4" s="0" t="s">
+      <c r="DA4" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="DB4" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="DC4" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="DD4" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="DE4" s="0" t="s">
-        <v>416</v>
-      </c>
-      <c r="DF4" s="0" t="s">
-        <v>417</v>
-      </c>
-      <c r="DG4" s="0" t="s">
-        <v>418</v>
-      </c>
-      <c r="DH4" s="0" t="s">
+      <c r="DE4" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="DI4" s="0" t="s">
+      <c r="DF4" s="2" t="s">
         <v>420</v>
       </c>
-      <c r="DJ4" s="0" t="s">
+      <c r="DG4" s="2" t="s">
         <v>421</v>
       </c>
-      <c r="DK4" s="0" t="s">
+      <c r="DH4" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="DI4" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="DJ4" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="DK4" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="DL4" s="0" t="s">
+      <c r="DL4" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="DM4" s="0" t="s">
+      <c r="DM4" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="DN4" s="0" t="s">
-        <v>422</v>
-      </c>
-      <c r="DO4" s="0" t="s">
+      <c r="DN4" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="DO4" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="DP4" s="0" t="s">
-        <v>423</v>
-      </c>
-      <c r="DQ4" s="0" t="s">
-        <v>424</v>
-      </c>
-      <c r="DR4" s="0" t="s">
-        <v>425</v>
-      </c>
-      <c r="DS4" s="0" t="s">
+      <c r="DP4" s="2" t="s">
         <v>426</v>
       </c>
-      <c r="DT4" s="0" t="s">
+      <c r="DQ4" s="2" t="s">
         <v>427</v>
       </c>
-      <c r="DU4" s="0" t="s">
+      <c r="DR4" s="2" t="s">
         <v>428</v>
       </c>
-      <c r="DV4" s="0" t="s">
+      <c r="DS4" s="2" t="s">
         <v>429</v>
       </c>
-      <c r="DW4" s="0" t="s">
+      <c r="DT4" s="2" t="s">
         <v>430</v>
       </c>
-      <c r="DX4" s="0" t="s">
+      <c r="DU4" s="2" t="s">
         <v>431</v>
       </c>
-      <c r="DY4" s="0" t="s">
+      <c r="DV4" s="2" t="s">
         <v>432</v>
       </c>
-      <c r="DZ4" s="0" t="s">
+      <c r="DW4" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="DX4" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="DY4" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="DZ4" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="EA4" s="0" t="s">
-        <v>433</v>
-      </c>
-      <c r="EB4" s="0" t="s">
-        <v>434</v>
-      </c>
-      <c r="EC4" s="0" t="s">
-        <v>435</v>
-      </c>
-      <c r="ED4" s="0" t="s">
+      <c r="EA4" s="2" t="s">
         <v>436</v>
       </c>
-      <c r="EE4" s="0" t="s">
+      <c r="EB4" s="2" t="s">
         <v>437</v>
       </c>
+      <c r="EC4" s="2" t="s">
+        <v>438</v>
+      </c>
+      <c r="ED4" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="EE4" s="2" t="s">
+        <v>440</v>
+      </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="0" t="n">
+    <row customHeight="1" ht="13.8" r="5" s="6" spans="1:200">
+      <c r="A5" t="s">
+        <v>441</v>
+      </c>
+      <c r="B5" s="2" t="n">
         <v>100</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>438</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="AE5" s="1" t="n">
+      <c r="C5" s="4" t="s">
+        <v>442</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="AE5" s="3" t="n">
         <v>400658</v>
       </c>
-      <c r="AJ5" s="1" t="s">
-        <v>439</v>
-      </c>
-      <c r="BB5" s="1" t="n">
+      <c r="AJ5" s="3" t="s">
+        <v>443</v>
+      </c>
+      <c r="BB5" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="BY5" s="1" t="n">
+      <c r="BY5" s="3" t="n">
         <v>35</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="0" t="n">
+    <row customHeight="1" ht="13.8" r="6" s="6" spans="1:200">
+      <c r="A6" t="s">
+        <v>444</v>
+      </c>
+      <c r="B6" s="2" t="n">
         <v>100</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>438</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="AE6" s="1" t="n">
+      <c r="C6" s="4" t="s">
+        <v>442</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="AE6" s="3" t="n">
         <v>400658</v>
       </c>
-      <c r="AJ6" s="1" t="s">
-        <v>440</v>
-      </c>
-      <c r="BB6" s="1"/>
-      <c r="BY6" s="1" t="n">
+      <c r="AJ6" s="3" t="s">
+        <v>445</v>
+      </c>
+      <c r="BB6" s="3" t="n"/>
+      <c r="BY6" s="3" t="n">
         <v>42</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="0" t="n">
+    <row customHeight="1" ht="13.8" r="7" s="6" spans="1:200">
+      <c r="A7" t="s">
+        <v>446</v>
+      </c>
+      <c r="B7" s="2" t="n">
         <v>100</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>438</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="AE7" s="1" t="n">
+      <c r="C7" s="4" t="s">
+        <v>442</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="AE7" s="3" t="n">
         <v>400658</v>
       </c>
-      <c r="AJ7" s="1" t="s">
-        <v>439</v>
-      </c>
-      <c r="BB7" s="1" t="n">
+      <c r="AJ7" s="3" t="s">
+        <v>443</v>
+      </c>
+      <c r="BB7" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="BY7" s="1" t="n">
+      <c r="BY7" s="3" t="n">
         <v>7</v>
       </c>
     </row>
+    <row r="8" spans="1:200"/>
+    <row r="9" spans="1:200"/>
+    <row r="10" spans="1:200"/>
+    <row r="11" spans="1:200"/>
+    <row r="12" spans="1:200"/>
+    <row r="13" spans="1:200"/>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageSetup blackAndWhite="0" copies="1" draft="0" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0" usePrinterDefaults="0" verticalDpi="300"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;K000000&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;K000000Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>